<commit_message>
tests for old pyene functionalities
</commit_message>
<xml_diff>
--- a/pyensys/tests/excel/excel_format_proposal.xlsx
+++ b/pyensys/tests/excel/excel_format_proposal.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f09903jm\OneDrive - The University of Manchester\Pyene\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f09903jm\git projects\pyensys\pyensys\tests\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="sheet6" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="129">
   <si>
     <t>DC Optimal Power Flow</t>
   </si>
@@ -178,18 +178,12 @@
     <t>T1</t>
   </si>
   <si>
-    <t>T2</t>
-  </si>
-  <si>
     <t>T3</t>
   </si>
   <si>
     <t>T4</t>
   </si>
   <si>
-    <t>T5</t>
-  </si>
-  <si>
     <t>T6</t>
   </si>
   <si>
@@ -373,18 +367,9 @@
     <t>type information</t>
   </si>
   <si>
-    <t>reference</t>
-  </si>
-  <si>
     <t>position tree</t>
   </si>
   <si>
-    <t>h5</t>
-  </si>
-  <si>
-    <t>sum</t>
-  </si>
-  <si>
     <t>data device</t>
   </si>
   <si>
@@ -394,12 +379,6 @@
     <t>none</t>
   </si>
   <si>
-    <t>surplus</t>
-  </si>
-  <si>
-    <t>parameters</t>
-  </si>
-  <si>
     <t>output file name</t>
   </si>
   <si>
@@ -409,9 +388,6 @@
     <t>excel</t>
   </si>
   <si>
-    <t>load curtailment</t>
-  </si>
-  <si>
     <t>wind</t>
   </si>
   <si>
@@ -431,6 +407,18 @@
   </si>
   <si>
     <t>representative periods</t>
+  </si>
+  <si>
+    <t>load curtailment</t>
+  </si>
+  <si>
+    <t>generation curtailment</t>
+  </si>
+  <si>
+    <t>PV1</t>
+  </si>
+  <si>
+    <t>W1</t>
   </si>
 </sst>
 </file>
@@ -768,24 +756,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.1796875" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" customWidth="1"/>
-    <col min="4" max="4" width="36.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
@@ -799,13 +787,13 @@
         <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -823,9 +811,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B4" s="1" t="b">
         <v>0</v>
@@ -834,46 +822,46 @@
         <v>12</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B5" s="1" t="b">
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="4" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="4" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -892,24 +880,24 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -917,7 +905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -928,12 +916,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -941,7 +929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -952,12 +940,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -965,7 +953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>2</v>
       </c>
@@ -976,12 +964,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>1</v>
       </c>
@@ -989,7 +977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>2</v>
       </c>
@@ -1009,30 +997,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y60"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1043,7 +1031,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1051,7 +1039,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1059,7 +1047,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1136,7 +1124,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1213,15 +1201,15 @@
         <v>0.49690000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1232,7 +1220,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1240,7 +1228,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1248,7 +1236,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1325,7 +1313,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1402,23 +1390,23 @@
         <v>0.40429999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1429,15 +1417,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1445,7 +1433,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1522,7 +1510,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -1599,23 +1587,23 @@
         <v>0.66600000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -1626,15 +1614,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -1642,7 +1630,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -1719,7 +1707,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -1796,23 +1784,23 @@
         <v>0.88500000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>2</v>
       </c>
       <c r="B42" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>31</v>
       </c>
       <c r="B43" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>30</v>
       </c>
@@ -1823,15 +1811,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>33</v>
       </c>
@@ -1839,7 +1827,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -1916,7 +1904,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>35</v>
       </c>
@@ -1993,23 +1981,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>2</v>
       </c>
       <c r="B54" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>31</v>
       </c>
       <c r="B55" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>30</v>
       </c>
@@ -2020,15 +2008,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>3</v>
       </c>
       <c r="B57" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>33</v>
       </c>
@@ -2036,7 +2024,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -2113,7 +2101,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>35</v>
       </c>
@@ -2201,38 +2189,38 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="2"/>
-    <col min="6" max="6" width="21.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.1796875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="17.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.1796875" style="2"/>
-    <col min="11" max="11" width="23.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="6" max="6" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="2"/>
+    <col min="11" max="11" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.1796875" style="2"/>
+    <col min="18" max="18" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2249,16 +2237,16 @@
         <v>19</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>6</v>
@@ -2282,22 +2270,22 @@
         <v>43</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -2362,15 +2350,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>48</v>
+        <v>128</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>46</v>
@@ -2427,9 +2415,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
@@ -2489,9 +2477,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="2">
         <v>3</v>
@@ -2554,15 +2542,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>51</v>
+        <v>127</v>
       </c>
       <c r="B7" s="2">
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E7" s="2">
         <v>1</v>
@@ -2616,9 +2604,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B8" s="2">
         <v>4</v>
@@ -2681,21 +2669,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
       </c>
       <c r="F9" s="2">
-        <v>700</v>
+        <v>100</v>
       </c>
       <c r="G9" s="2">
         <v>0</v>
@@ -2743,21 +2731,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B10" s="2">
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E10" s="2">
         <v>2</v>
       </c>
       <c r="F10" s="2">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="G10" s="2">
         <v>0</v>
@@ -2818,28 +2806,28 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.453125" customWidth="1"/>
-    <col min="10" max="10" width="28.453125" customWidth="1"/>
-    <col min="11" max="11" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="28.42578125" customWidth="1"/>
+    <col min="11" max="11" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2850,34 +2838,34 @@
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>18</v>
@@ -2889,12 +2877,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2936,12 +2924,12 @@
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -2986,15 +2974,15 @@
         <v>1</v>
       </c>
       <c r="P4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -3036,15 +3024,15 @@
         <v>1</v>
       </c>
       <c r="P5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -3086,7 +3074,7 @@
         <v>1</v>
       </c>
       <c r="P6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -3103,20 +3091,20 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -3124,7 +3112,7 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -3138,16 +3126,16 @@
         <v>31</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>6</v>
@@ -3156,15 +3144,15 @@
         <v>15</v>
       </c>
       <c r="K2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3200,9 +3188,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3238,9 +3226,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3276,9 +3264,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3314,9 +3302,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3352,9 +3340,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3390,9 +3378,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -3428,9 +3416,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -3466,9 +3454,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -3517,62 +3505,62 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -3580,17 +3568,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
     </row>
   </sheetData>
@@ -3604,28 +3592,28 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -3633,13 +3621,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" t="s">
         <v>108</v>
       </c>
-      <c r="D4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -3659,12 +3647,12 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -3679,12 +3667,12 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -3699,12 +3687,12 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -3719,50 +3707,16 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>2</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17">
-        <v>3</v>
-      </c>
-      <c r="D17">
-        <v>30</v>
-      </c>
-      <c r="E17">
-        <v>10</v>
-      </c>
-      <c r="F17">
-        <v>2800</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>2</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="D18">
-        <v>60</v>
-      </c>
-      <c r="E18">
-        <v>300</v>
-      </c>
-      <c r="F18">
-        <v>2200</v>
-      </c>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3773,782 +3727,459 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C109"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="G83" sqref="G83"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B9" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C39" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
-        <v>101</v>
-      </c>
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="2" t="s">
-        <v>31</v>
-      </c>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" s="2" t="s">
-        <v>19</v>
-      </c>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
       <c r="B49" s="2"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" s="2" t="s">
-        <v>18</v>
-      </c>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" s="2" t="s">
-        <v>101</v>
-      </c>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
       <c r="B59" s="2"/>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" s="2" t="s">
-        <v>31</v>
-      </c>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
       <c r="B63" s="2"/>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" s="2" t="s">
-        <v>19</v>
-      </c>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
       <c r="B64" s="2"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" s="2" t="s">
-        <v>18</v>
-      </c>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
       <c r="B65" s="2"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C70" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B75" s="2"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A76" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A77" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C82" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B87" s="2"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A89" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C94" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A99" s="2" t="s">
-        <v>101</v>
-      </c>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="2"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="2"/>
       <c r="B99" s="2"/>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A100" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A103" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A104" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A105" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A106" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A107" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A108" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A109" s="2" t="s">
-        <v>102</v>
-      </c>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="2"/>
+      <c r="B100" s="2"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="2"/>
+      <c r="B101" s="2"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="2"/>
+      <c r="B102" s="2"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="2"/>
+      <c r="B103" s="2"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="2"/>
+      <c r="B104" s="2"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="2"/>
+      <c r="B105" s="2"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
+      <c r="B106" s="2"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="2"/>
+      <c r="B107" s="2"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="2"/>
+      <c r="B108" s="2"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004626D7760A3C1F469AFD6100FC26A4FC" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="034eb952937b7235f0911bdae931632f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ef315e9c-09f6-4f08-8f36-bc97357cd5f0" xmlns:ns4="68c75d18-20a7-4f69-86ec-e9bf7e3de19a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1eaa6ff1e0ef27472ec4646cc52f33dd" ns3:_="" ns4:_="">
     <xsd:import namespace="ef315e9c-09f6-4f08-8f36-bc97357cd5f0"/>
@@ -4771,10 +4402,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5A4238A-6E06-4EAC-A00B-316A1A8A888C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F831E3D6-AA23-4539-B083-2A305CA51B4B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ef315e9c-09f6-4f08-8f36-bc97357cd5f0"/>
+    <ds:schemaRef ds:uri="68c75d18-20a7-4f69-86ec-e9bf7e3de19a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4797,20 +4454,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F831E3D6-AA23-4539-B083-2A305CA51B4B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5A4238A-6E06-4EAC-A00B-316A1A8A888C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ef315e9c-09f6-4f08-8f36-bc97357cd5f0"/>
-    <ds:schemaRef ds:uri="68c75d18-20a7-4f69-86ec-e9bf7e3de19a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>